<commit_message>
Refactor: Restructure main program architecture for better modularity
</commit_message>
<xml_diff>
--- a/template/employee_report_template.xlsx
+++ b/template/employee_report_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ythsi\Pycharm\AttendanceProject\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B60122-8C34-4212-BDD5-EC8CDD92CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38337295-D69B-4BCB-8E43-216745C03BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AEB25E42-977A-4128-95ED-AE51CD6399DB}"/>
   </bookViews>
@@ -477,10 +477,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,6 +580,16 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,12 +608,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1012,7 +1014,7 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,19 +1034,19 @@
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="28" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="H1" s="28" t="s">
+      <c r="F1" s="43"/>
+      <c r="H1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="49"/>
+      <c r="I1" s="47"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1059,19 +1061,19 @@
     </row>
     <row r="2" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4"/>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="29" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="44"/>
+      <c r="H2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="50"/>
+      <c r="I2" s="48"/>
       <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1086,40 +1088,40 @@
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="44" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="H3" s="28" t="s">
+      <c r="F3" s="45"/>
+      <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="50"/>
+      <c r="I3" s="48"/>
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="2"/>
-      <c r="R3" s="54"/>
+      <c r="R3" s="52"/>
     </row>
     <row r="4" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="5"/>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="51"/>
+      <c r="I4" s="49"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1133,13 +1135,13 @@
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="30" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="26"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="24"/>
       <c r="K5" s="6"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -1153,11 +1155,11 @@
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="53"/>
-      <c r="J6" s="26"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1181,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="12"/>
       <c r="K7" s="2"/>
       <c r="L7" s="3"/>
@@ -1201,15 +1203,15 @@
       <c r="A9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="14"/>
       <c r="G9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="56"/>
       <c r="I9" t="s">
         <v>19</v>
       </c>
@@ -1217,15 +1219,15 @@
       <c r="K9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="15"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1233,836 +1235,837 @@
       <c r="C10" s="5"/>
       <c r="F10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="N10" s="34" t="b">
+      <c r="N10" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="O10" s="61"/>
-      <c r="P10" s="18"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="16"/>
     </row>
     <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N11" s="35" t="s">
+      <c r="N11" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="Q11" s="22" t="s">
+      <c r="Q11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="55"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="57"/>
     </row>
     <row r="13" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="56"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="58"/>
     </row>
     <row r="14" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="56"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="58"/>
     </row>
     <row r="15" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="56"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="58"/>
     </row>
     <row r="16" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="56"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="58"/>
     </row>
     <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="56"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="58"/>
     </row>
     <row r="18" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="56"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="58"/>
     </row>
     <row r="19" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="56"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="58"/>
     </row>
     <row r="20" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="56"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="58"/>
     </row>
     <row r="21" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="56"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="58"/>
     </row>
     <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="56"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="58"/>
     </row>
     <row r="23" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="56"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="58"/>
     </row>
     <row r="24" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="56"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="58"/>
     </row>
     <row r="25" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="56"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="58"/>
     </row>
     <row r="26" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="56"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="58"/>
     </row>
     <row r="27" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="56"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="58"/>
     </row>
     <row r="28" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="56"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="58"/>
     </row>
     <row r="29" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="56"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="58"/>
     </row>
     <row r="30" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="56"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="58"/>
     </row>
     <row r="31" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="56"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="58"/>
     </row>
     <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="56"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="58"/>
     </row>
     <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="56"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="58"/>
     </row>
     <row r="34" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="63"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="56"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="58"/>
     </row>
     <row r="35" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="56"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="54"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="58"/>
     </row>
     <row r="36" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="38"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="56"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="58"/>
     </row>
     <row r="37" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="56"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="58"/>
     </row>
     <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="38"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="56"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="58"/>
     </row>
     <row r="39" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="38"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="56"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="58"/>
     </row>
     <row r="40" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="38"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="56"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="58"/>
     </row>
     <row r="41" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="56"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="58"/>
     </row>
     <row r="42" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="56"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="36"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="58"/>
     </row>
     <row r="43" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="56"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="40"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="58"/>
     </row>
     <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="25"/>
-      <c r="R44" s="56"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="36"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="58"/>
     </row>
     <row r="45" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="38"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="56"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="40"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="58"/>
     </row>
     <row r="46" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A46" s="23"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="56"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="55"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="58"/>
     </row>
     <row r="47" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="42"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="56"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="58"/>
     </row>
     <row r="48" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="56"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="58"/>
     </row>
     <row r="49" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="42"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="56"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="30"/>
+      <c r="R49" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="R12:R49"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="Q9:R9"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>